<commit_message>
implemented the ROW() function (so long as it can be replaced at runtime) and implemented the COLUMN() function without arguments
</commit_message>
<xml_diff>
--- a/examples/eu.xlsx
+++ b/examples/eu.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="220" windowWidth="12220" windowHeight="9700"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480"/>
   </bookViews>
   <sheets>
     <sheet name="EU" sheetId="1" r:id="rId1"/>
     <sheet name="OLD UK" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="130407" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -270,11 +270,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -363,10 +363,10 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -375,7 +375,7 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -431,15 +431,25 @@
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:style val="2"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -455,6 +465,7 @@
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
@@ -480,6 +491,7 @@
               <a:prstDash val="solid"/>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>EU!$F$27:$M$27</c:f>
@@ -572,6 +584,7 @@
               <a:prstDash val="solid"/>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>EU!$F$27:$M$27</c:f>
@@ -639,12 +652,22 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="575712280"/>
-        <c:axId val="537868520"/>
+        <c:axId val="1794052856"/>
+        <c:axId val="1794048008"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="2"/>
@@ -703,18 +726,31 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="575712280"/>
-        <c:axId val="537868520"/>
+        <c:smooth val="0"/>
+        <c:axId val="1794052856"/>
+        <c:axId val="1794048008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="575712280"/>
+        <c:axId val="1794052856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln w="3175">
@@ -741,20 +777,22 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="537868520"/>
+        <c:crossAx val="1794048008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="537868520"/>
+        <c:axId val="1794048008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="35.0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -797,6 +835,7 @@
               <c:y val="0.252841259822859"/>
             </c:manualLayout>
           </c:layout>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln w="25400">
@@ -805,6 +844,8 @@
           </c:spPr>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln w="3175">
@@ -831,7 +872,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="575712280"/>
+        <c:crossAx val="1794052856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -854,6 +895,7 @@
           <c:h val="0.190341173125074"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
@@ -885,6 +927,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -921,9 +964,19 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:style val="2"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -939,6 +992,7 @@
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
@@ -964,6 +1018,7 @@
               <a:prstDash val="solid"/>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'OLD UK'!$C$17:$J$17</c:f>
@@ -1056,6 +1111,7 @@
               <a:prstDash val="solid"/>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'OLD UK'!$C$17:$J$17</c:f>
@@ -1123,17 +1179,29 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="575782088"/>
-        <c:axId val="575786776"/>
+        <c:axId val="-2129028072"/>
+        <c:axId val="-2129019688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="575782088"/>
+        <c:axId val="-2129028072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln w="3175">
@@ -1160,19 +1228,21 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="575786776"/>
+        <c:crossAx val="-2129019688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="575786776"/>
+        <c:axId val="-2129019688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1215,6 +1285,7 @@
               <c:y val="0.199186893029243"/>
             </c:manualLayout>
           </c:layout>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln w="25400">
@@ -1223,6 +1294,8 @@
           </c:spPr>
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln w="3175">
@@ -1249,7 +1322,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="575782088"/>
+        <c:crossAx val="-2129028072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1272,6 +1345,7 @@
           <c:h val="0.126016197630745"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
@@ -1303,6 +1377,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1828,14 +1903,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="B1:P46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:Q48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" topLeftCell="N22" workbookViewId="0">
+      <selection activeCell="P46" sqref="P46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="2.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="28.42578125" style="1" customWidth="1"/>
@@ -2935,7 +3010,7 @@
       <c r="M32" s="17"/>
       <c r="N32" s="11"/>
     </row>
-    <row r="33" spans="2:14">
+    <row r="33" spans="2:17">
       <c r="B33" s="39" t="s">
         <v>42</v>
       </c>
@@ -2952,7 +3027,7 @@
       <c r="M33" s="17"/>
       <c r="N33" s="11"/>
     </row>
-    <row r="34" spans="2:14">
+    <row r="34" spans="2:17">
       <c r="B34" s="11" t="s">
         <v>0</v>
       </c>
@@ -2993,7 +3068,7 @@
       </c>
       <c r="N34" s="11"/>
     </row>
-    <row r="35" spans="2:14">
+    <row r="35" spans="2:17">
       <c r="B35" s="11" t="s">
         <v>39</v>
       </c>
@@ -3034,7 +3109,7 @@
       </c>
       <c r="N35" s="11"/>
     </row>
-    <row r="36" spans="2:14">
+    <row r="36" spans="2:17">
       <c r="B36" s="11"/>
       <c r="C36" s="11"/>
       <c r="D36" s="11"/>
@@ -3049,7 +3124,7 @@
       <c r="M36" s="17"/>
       <c r="N36" s="11"/>
     </row>
-    <row r="37" spans="2:14">
+    <row r="37" spans="2:17">
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
       <c r="D37" s="11"/>
@@ -3064,7 +3139,7 @@
       <c r="M37" s="17"/>
       <c r="N37" s="11"/>
     </row>
-    <row r="39" spans="2:14">
+    <row r="39" spans="2:17">
       <c r="B39" s="1" t="s">
         <v>17</v>
       </c>
@@ -3079,7 +3154,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="2:14">
+    <row r="40" spans="2:17">
       <c r="B40" s="1" t="s">
         <v>18</v>
       </c>
@@ -3090,7 +3165,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="2:14">
+    <row r="41" spans="2:17">
       <c r="B41" s="1" t="s">
         <v>19</v>
       </c>
@@ -3099,7 +3174,7 @@
         <v>0.13557422969187674</v>
       </c>
     </row>
-    <row r="42" spans="2:14">
+    <row r="42" spans="2:17">
       <c r="B42" s="1" t="s">
         <v>20</v>
       </c>
@@ -3107,7 +3182,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="43" spans="2:14">
+    <row r="43" spans="2:17">
       <c r="B43" s="1" t="s">
         <v>21</v>
       </c>
@@ -3116,7 +3191,7 @@
         <v>0.12201680672268907</v>
       </c>
     </row>
-    <row r="45" spans="2:14">
+    <row r="45" spans="2:17">
       <c r="B45" s="7" t="s">
         <v>22</v>
       </c>
@@ -3157,7 +3232,7 @@
       </c>
       <c r="N45" s="7"/>
     </row>
-    <row r="46" spans="2:14">
+    <row r="46" spans="2:17">
       <c r="B46" s="13" t="s">
         <v>2</v>
       </c>
@@ -3199,15 +3274,30 @@
       <c r="N46" s="13" t="s">
         <v>11</v>
       </c>
+      <c r="Q46" s="1">
+        <f>COLUMN()+ROW()</f>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="47" spans="2:17">
+      <c r="Q47" s="1">
+        <f>ROW()</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="2:17">
+      <c r="Q48" s="1">
+        <f>COLUMN()</f>
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -3215,14 +3305,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="2.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -3353,7 +3443,7 @@
       </c>
       <c r="L6" s="25">
         <f>-((J6/C6)^(1/(J4-C4))-1)</f>
-        <v>1.7400000000000082E-2</v>
+        <v>1.7399999999999971E-2</v>
       </c>
     </row>
     <row r="7" spans="2:12">
@@ -3797,13 +3887,12 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
Implemented the EXP function in ruby and C
</commit_message>
<xml_diff>
--- a/examples/eu.xlsx
+++ b/examples/eu.xlsx
@@ -662,8 +662,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="1794052856"/>
-        <c:axId val="1794048008"/>
+        <c:axId val="1812902024"/>
+        <c:axId val="1812904632"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -738,11 +738,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1794052856"/>
-        <c:axId val="1794048008"/>
+        <c:axId val="1812902024"/>
+        <c:axId val="1812904632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1794052856"/>
+        <c:axId val="1812902024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -777,7 +777,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1794048008"/>
+        <c:crossAx val="1812904632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -787,7 +787,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1794048008"/>
+        <c:axId val="1812904632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="35.0"/>
@@ -872,7 +872,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1794052856"/>
+        <c:crossAx val="1812902024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1189,11 +1189,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2129028072"/>
-        <c:axId val="-2129019688"/>
+        <c:axId val="1812073832"/>
+        <c:axId val="1812057752"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2129028072"/>
+        <c:axId val="1812073832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1228,7 +1228,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2129019688"/>
+        <c:crossAx val="1812057752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1238,7 +1238,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2129019688"/>
+        <c:axId val="1812057752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1322,7 +1322,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2129028072"/>
+        <c:crossAx val="1812073832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1907,7 +1907,7 @@
   <dimension ref="B1:Q48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="N22" workbookViewId="0">
-      <selection activeCell="P46" sqref="P46"/>
+      <selection activeCell="Q44" sqref="Q44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -1917,7 +1917,9 @@
     <col min="3" max="3" width="8.140625" style="1" customWidth="1"/>
     <col min="4" max="5" width="9.7109375" style="1" customWidth="1"/>
     <col min="6" max="13" width="6.42578125" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.7109375" style="1"/>
+    <col min="14" max="16" width="8.7109375" style="1"/>
+    <col min="17" max="17" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:15">
@@ -3189,6 +3191,12 @@
       <c r="F43" s="2">
         <f>F42*F41</f>
         <v>0.12201680672268907</v>
+      </c>
+    </row>
+    <row r="44" spans="2:17">
+      <c r="Q44" s="1">
+        <f>1-EXP(Q46)</f>
+        <v>-2.29378315946961E+27</v>
       </c>
     </row>
     <row r="45" spans="2:17">

</xml_diff>

<commit_message>
implemented the TRANSPOSE function (removed at compile time, only works in array formulae)
</commit_message>
<xml_diff>
--- a/examples/eu.xlsx
+++ b/examples/eu.xlsx
@@ -10,6 +10,9 @@
     <sheet name="EU" sheetId="1" r:id="rId1"/>
     <sheet name="OLD UK" sheetId="4" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="some_row_names">EU!$B$33:$B$35</definedName>
+  </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -662,8 +665,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="1812902024"/>
-        <c:axId val="1812904632"/>
+        <c:axId val="2065436712"/>
+        <c:axId val="2065459288"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -738,11 +741,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1812902024"/>
-        <c:axId val="1812904632"/>
+        <c:axId val="2065436712"/>
+        <c:axId val="2065459288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1812902024"/>
+        <c:axId val="2065436712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -777,7 +780,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1812904632"/>
+        <c:crossAx val="2065459288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -787,7 +790,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1812904632"/>
+        <c:axId val="2065459288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="35.0"/>
@@ -872,7 +875,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1812902024"/>
+        <c:crossAx val="2065436712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1189,11 +1192,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="1812073832"/>
-        <c:axId val="1812057752"/>
+        <c:axId val="-2059803576"/>
+        <c:axId val="2136093512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1812073832"/>
+        <c:axId val="-2059803576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1228,7 +1231,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1812057752"/>
+        <c:crossAx val="2136093512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1238,7 +1241,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1812057752"/>
+        <c:axId val="2136093512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1322,7 +1325,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1812073832"/>
+        <c:crossAx val="-2059803576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1906,8 +1909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Q48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N22" workbookViewId="0">
-      <selection activeCell="Q44" sqref="Q44"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -3127,9 +3130,16 @@
       <c r="N36" s="11"/>
     </row>
     <row r="37" spans="2:17">
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
+      <c r="B37" s="11" t="str">
+        <f t="array" ref="B37:D37">TRANSPOSE(some_row_names)</f>
+        <v>Revenues</v>
+      </c>
+      <c r="C37" s="11" t="str">
+        <v>Power sector</v>
+      </c>
+      <c r="D37" s="11" t="str">
+        <v>Other sectors</v>
+      </c>
       <c r="E37" s="11"/>
       <c r="F37" s="17"/>
       <c r="G37" s="17"/>

</xml_diff>

<commit_message>
Now aborts earlier in the process if the spreadsheet contains functions that haven't yet been implemented in excel_to_code
</commit_message>
<xml_diff>
--- a/examples/eu.xlsx
+++ b/examples/eu.xlsx
@@ -665,8 +665,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2065436712"/>
-        <c:axId val="2065459288"/>
+        <c:axId val="2119749816"/>
+        <c:axId val="2119753224"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -741,11 +741,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2065436712"/>
-        <c:axId val="2065459288"/>
+        <c:axId val="2119749816"/>
+        <c:axId val="2119753224"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2065436712"/>
+        <c:axId val="2119749816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -780,7 +780,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2065459288"/>
+        <c:crossAx val="2119753224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -790,7 +790,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2065459288"/>
+        <c:axId val="2119753224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="35.0"/>
@@ -875,7 +875,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2065436712"/>
+        <c:crossAx val="2119749816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1192,11 +1192,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2059803576"/>
-        <c:axId val="2136093512"/>
+        <c:axId val="2119806824"/>
+        <c:axId val="2119810248"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2059803576"/>
+        <c:axId val="2119806824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1231,7 +1231,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2136093512"/>
+        <c:crossAx val="2119810248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1241,7 +1241,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2136093512"/>
+        <c:axId val="2119810248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1325,7 +1325,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2059803576"/>
+        <c:crossAx val="2119806824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1910,7 +1910,7 @@
   <dimension ref="B1:Q48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="O37" sqref="O37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Implemented the AVERAGEIFS function
</commit_message>
<xml_diff>
--- a/examples/eu.xlsx
+++ b/examples/eu.xlsx
@@ -665,8 +665,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2119749816"/>
-        <c:axId val="2119753224"/>
+        <c:axId val="2118647928"/>
+        <c:axId val="2118651336"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -741,11 +741,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2119749816"/>
-        <c:axId val="2119753224"/>
+        <c:axId val="2118647928"/>
+        <c:axId val="2118651336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2119749816"/>
+        <c:axId val="2118647928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -780,7 +780,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2119753224"/>
+        <c:crossAx val="2118651336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -790,7 +790,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2119753224"/>
+        <c:axId val="2118651336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="35.0"/>
@@ -875,7 +875,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2119749816"/>
+        <c:crossAx val="2118647928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1192,11 +1192,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2119806824"/>
-        <c:axId val="2119810248"/>
+        <c:axId val="2118704936"/>
+        <c:axId val="2118708360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2119806824"/>
+        <c:axId val="2118704936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1231,7 +1231,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2119810248"/>
+        <c:crossAx val="2118708360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1241,7 +1241,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2119810248"/>
+        <c:axId val="2118708360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1325,7 +1325,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2119806824"/>
+        <c:crossAx val="2118704936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3150,6 +3150,10 @@
       <c r="L37" s="17"/>
       <c r="M37" s="17"/>
       <c r="N37" s="11"/>
+      <c r="O37" s="1">
+        <f>AVERAGEIFS(F34:M34,F27:M27,"&gt;1")</f>
+        <v>30321.091534806292</v>
+      </c>
     </row>
     <row r="39" spans="2:17">
       <c r="B39" s="1" t="s">

</xml_diff>

<commit_message>
Implemented the FORECAST function
</commit_message>
<xml_diff>
--- a/examples/eu.xlsx
+++ b/examples/eu.xlsx
@@ -1910,7 +1910,7 @@
   <dimension ref="B1:Q48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="O37" sqref="O37"/>
+      <selection activeCell="P34" sqref="P34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -3072,6 +3072,10 @@
         <v>33737.604819435837</v>
       </c>
       <c r="N34" s="11"/>
+      <c r="P34" s="1">
+        <f>FORECAST(40000,F34:M34,F35:M35)</f>
+        <v>39117.488088819038</v>
+      </c>
     </row>
     <row r="35" spans="2:17">
       <c r="B35" s="11" t="s">

</xml_diff>

<commit_message>
Fix SUBTOTAL to not count other SUBTOTALs
</commit_message>
<xml_diff>
--- a/examples/eu.xlsx
+++ b/examples/eu.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="21721"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="EU" sheetId="1" r:id="rId1"/>
     <sheet name="OLD UK" sheetId="4" r:id="rId2"/>
+    <sheet name="subtotals" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="some_row_names">EU!$B$33:$B$35</definedName>
@@ -665,8 +666,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2118647928"/>
-        <c:axId val="2118651336"/>
+        <c:axId val="2138863320"/>
+        <c:axId val="2138866664"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -741,11 +742,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2118647928"/>
-        <c:axId val="2118651336"/>
+        <c:axId val="2138863320"/>
+        <c:axId val="2138866664"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2118647928"/>
+        <c:axId val="2138863320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -780,7 +781,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2118651336"/>
+        <c:crossAx val="2138866664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -790,7 +791,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2118651336"/>
+        <c:axId val="2138866664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="35.0"/>
@@ -875,7 +876,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2118647928"/>
+        <c:crossAx val="2138863320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1192,11 +1193,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2118704936"/>
-        <c:axId val="2118708360"/>
+        <c:axId val="2131128184"/>
+        <c:axId val="2111507384"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2118704936"/>
+        <c:axId val="2131128184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1231,7 +1232,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2118708360"/>
+        <c:crossAx val="2111507384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1241,7 +1242,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2118708360"/>
+        <c:axId val="2111507384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1325,7 +1326,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2118704936"/>
+        <c:crossAx val="2131128184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1909,7 +1910,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Q48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="P34" sqref="P34"/>
     </sheetView>
   </sheetViews>
@@ -3923,4 +3924,72 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="3" spans="2:2">
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2">
+      <c r="B4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2">
+      <c r="B5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2">
+      <c r="B6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2">
+      <c r="B7">
+        <f>SUBTOTAL(109,B5:B6,B3:B4)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2">
+      <c r="B8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2">
+      <c r="B9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2">
+      <c r="B10">
+        <f>SUBTOTAL(109,B9,B8,B7,B6,B5,B4,B3)</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2">
+      <c r="B11">
+        <f>SUBTOTAL(109,B3:B10)</f>
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>